<commit_message>
Added suggested format for raw results table.
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MONICA\Documents\GitHub\projectpaper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="2" r:id="rId1"/>
     <sheet name="Drozer" sheetId="3" r:id="rId2"/>
     <sheet name="Androbugs" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="184">
   <si>
     <t>Runtime Command Checking</t>
   </si>
@@ -582,6 +578,27 @@
   <si>
     <t>Application</t>
   </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Priority Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem </t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TSB</t>
+  </si>
 </sst>
 </file>
 
@@ -751,7 +768,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -786,7 +803,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -963,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1296,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EM162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8124,7 +8141,7 @@
       <c r="EL45" s="7"/>
       <c r="EM45" s="7"/>
     </row>
-    <row r="46" spans="1:143" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:143" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="10" t="s">
         <v>35</v>
@@ -25185,4 +25202,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="33.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>